<commit_message>
modifying Accenture.py file, still need to finish Selenium stuff
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>titles</t>
   </si>
@@ -28,16 +28,136 @@
     <t>date_listed</t>
   </si>
   <si>
+    <t>newData Science Internship (Philadelphia) - Publicis Health</t>
+  </si>
+  <si>
+    <t>newData Analytics Intern (Summer 2022)</t>
+  </si>
+  <si>
     <t>newSummer 2022 Data Science Intern</t>
   </si>
   <si>
+    <t>newData Science Summer Intern - AI Innovations</t>
+  </si>
+  <si>
+    <t>newResearch/Data Scientist Intern</t>
+  </si>
+  <si>
+    <t>newIntern - IT Data &amp; Analytics</t>
+  </si>
+  <si>
+    <t>newHR Intern, People Analytics (Summer)</t>
+  </si>
+  <si>
+    <t>newData Science Intern</t>
+  </si>
+  <si>
+    <t>newInventory Planning &amp; Business Analytics Intern</t>
+  </si>
+  <si>
+    <t>newPaid Internship - IT/Tech</t>
+  </si>
+  <si>
+    <t>newData Center Platform Application Engineer Intern</t>
+  </si>
+  <si>
+    <t>newIOTG Research AI Scientist internship</t>
+  </si>
+  <si>
+    <t>newIntern - Data Science</t>
+  </si>
+  <si>
+    <t>newIntern: Energy Trading Analyst</t>
+  </si>
+  <si>
+    <t>Publicis Health</t>
+  </si>
+  <si>
+    <t>Poshmark</t>
+  </si>
+  <si>
     <t>Slack</t>
   </si>
   <si>
-    <t>www.indeed.com//rc/clk?jk=42264fe69e4da293&amp;fccid=8d0ce3817d129779&amp;vjs=3</t>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>Ascension</t>
+  </si>
+  <si>
+    <t>Amcor</t>
+  </si>
+  <si>
+    <t>TriNet</t>
+  </si>
+  <si>
+    <t>Varian Medical Systems</t>
+  </si>
+  <si>
+    <t>Fullbeauty</t>
+  </si>
+  <si>
+    <t>The Shopping Center Group</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>Navistar, Inc.</t>
+  </si>
+  <si>
+    <t>Greenwich Commodities LLC</t>
+  </si>
+  <si>
+    <t>Meketa Investment Group</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Publicis-Healthcare-Communications-Group</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Poshmark</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Slack</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/IBM</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Ascension</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Amcor</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Trinet</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Varian-Medical-Systems</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Fullbeauty</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/The-Shopping-Center-Group</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Intel-Corporation</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Navistar,-Inc.</t>
+  </si>
+  <si>
+    <t>www.indeed.com//jobs?q=Greenwich+Commodities+LLC&amp;l=Denver,+CO&amp;nc=jasx</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Meketa-Investment-Group</t>
   </si>
   <si>
     <t>PostedJust posted</t>
+  </si>
+  <si>
+    <t>PostedToday</t>
   </si>
 </sst>
 </file>
@@ -395,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,13 +543,251 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created working L3Harris file, needs to be customized later depending on how we want to import data to the website
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>titles</t>
   </si>
@@ -28,16 +28,124 @@
     <t>date_listed</t>
   </si>
   <si>
+    <t>new2022 Summer Data Analyst Intern</t>
+  </si>
+  <si>
+    <t>newFX Data Analytics Internship, Remote, Summer/Fall 2022</t>
+  </si>
+  <si>
+    <t>newData Center Platform Application Engineer Intern</t>
+  </si>
+  <si>
+    <t>new2022 Summer PHD Data Analytics Research Intern</t>
+  </si>
+  <si>
+    <t>newDeep Learning Software Engineer Graduate Internship</t>
+  </si>
+  <si>
+    <t>newIOTG Research AI Scientist internship</t>
+  </si>
+  <si>
     <t>newSummer 2022 Data Science Intern</t>
   </si>
   <si>
+    <t>newData Science Internship (Philadelphia) - Publicis Health</t>
+  </si>
+  <si>
+    <t>newInventory Planning &amp; Business Analytics Intern</t>
+  </si>
+  <si>
+    <t>newData Science Summer Intern - AI Innovations</t>
+  </si>
+  <si>
+    <t>newData Analytics Intern (Summer 2022)</t>
+  </si>
+  <si>
+    <t>newResearch/Data Scientist Intern</t>
+  </si>
+  <si>
+    <t>newData Science Intern</t>
+  </si>
+  <si>
+    <t>newJunior Business Analyst Intern</t>
+  </si>
+  <si>
+    <t>newIntern: Energy Trading Analyst</t>
+  </si>
+  <si>
+    <t>General Motors</t>
+  </si>
+  <si>
+    <t>General Entertainment Content</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
     <t>Slack</t>
   </si>
   <si>
-    <t>www.indeed.com//rc/clk?jk=42264fe69e4da293&amp;fccid=8d0ce3817d129779&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>PostedJust posted</t>
+    <t>Publicis Health</t>
+  </si>
+  <si>
+    <t>Fullbeauty</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>Poshmark</t>
+  </si>
+  <si>
+    <t>Ascension</t>
+  </si>
+  <si>
+    <t>Varian Medical Systems</t>
+  </si>
+  <si>
+    <t>Elsevier</t>
+  </si>
+  <si>
+    <t>Greenwich Commodities LLC</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/General-Motors</t>
+  </si>
+  <si>
+    <t>www.indeed.com//q-General-Entertainment-Content-l-Burbank,-CA-jobs.html</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Intel-Corporation</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Slack</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Publicis-Healthcare-Communications-Group</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Fullbeauty</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/IBM</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Poshmark</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Ascension</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Varian-Medical-Systems</t>
+  </si>
+  <si>
+    <t>www.indeed.com//cmp/Relx-Group</t>
+  </si>
+  <si>
+    <t>www.indeed.com//jobs?q=Greenwich+Commodities+LLC&amp;l=Denver,+CO&amp;nc=jasx</t>
+  </si>
+  <si>
+    <t>PostedToday</t>
   </si>
 </sst>
 </file>
@@ -395,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,13 +531,251 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>